<commit_message>
Update db parameters for freq reg demo
</commit_message>
<xml_diff>
--- a/demo/freq_regulation/ieee39_dyn.xlsx
+++ b/demo/freq_regulation/ieee39_dyn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/demo/demo/freq_regulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB682FBE-0F52-7646-B634-46253281382D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1CB576-8E4D-A940-B585-CAF9E189CC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="700" windowWidth="21600" windowHeight="18940" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="700" windowWidth="21600" windowHeight="18940" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Line" sheetId="7" r:id="rId6"/>
     <sheet name="Area" sheetId="8" r:id="rId7"/>
     <sheet name="GENROU" sheetId="9" r:id="rId8"/>
-    <sheet name="TGOV1N" sheetId="10" r:id="rId9"/>
+    <sheet name="TGOV1DB" sheetId="10" r:id="rId9"/>
     <sheet name="IEEEX1" sheetId="11" r:id="rId10"/>
     <sheet name="IEEEST" sheetId="12" r:id="rId11"/>
     <sheet name="BusFreq" sheetId="13" r:id="rId12"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3464" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3466" uniqueCount="829">
   <si>
     <t>uid</t>
   </si>
@@ -2515,6 +2515,12 @@
   </si>
   <si>
     <t>BusFreq_39</t>
+  </si>
+  <si>
+    <t>dbL</t>
+  </si>
+  <si>
+    <t>dbU</t>
   </si>
 </sst>
 </file>
@@ -13506,15 +13512,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13557,8 +13563,14 @@
       <c r="N1" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" t="s">
+        <v>827</v>
+      </c>
+      <c r="P1" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -13598,8 +13610,14 @@
       <c r="N2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="P2">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -13639,8 +13657,14 @@
       <c r="N3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="P3">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -13680,8 +13704,14 @@
       <c r="N4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="P4">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -13721,8 +13751,14 @@
       <c r="N5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="P5">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -13762,8 +13798,14 @@
       <c r="N6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="P6">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -13803,8 +13845,14 @@
       <c r="N7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="P7">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -13844,8 +13892,14 @@
       <c r="N8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="P8">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -13885,8 +13939,14 @@
       <c r="N9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="P9">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -13926,8 +13986,14 @@
       <c r="N10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="P10">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -13966,6 +14032,12 @@
       </c>
       <c r="N11" t="s">
         <v>14</v>
+      </c>
+      <c r="O11">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="P11">
+        <v>5.9999999999999995E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>